<commit_message>
export tables to csv
</commit_message>
<xml_diff>
--- a/tables/Simulatoren.xlsx
+++ b/tables/Simulatoren.xlsx
@@ -1286,58 +1286,58 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="2" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="3" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="3" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="5" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="6" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="7" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="3" fillId="0" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="9" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="10" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="11" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="3" fillId="0" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="13" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="14" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1900,7 +1900,7 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.333300000000001" defaultRowHeight="19.899999999999999" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="16.333300000000001" defaultRowHeight="12.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" style="1" width="5.3828100000000001"/>
     <col customWidth="1" min="2" max="6" style="1" width="16.351600000000001"/>
@@ -1910,7 +1910,7 @@
     <col customWidth="1" min="20" max="16384" style="1" width="16.351600000000001"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.449999999999999" customHeight="1">
+    <row r="1" ht="19.899999999999999">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" ht="68.450000000000003" customHeight="1">
+    <row r="2" ht="13.5">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" ht="44.200000000000003" customHeight="1">
+    <row r="3" ht="13.5">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" ht="68.200000000000003" customHeight="1">
+    <row r="4" ht="13.5">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" ht="44.200000000000003" customHeight="1">
+    <row r="5" ht="13.5">
       <c r="A5" s="10">
         <v>4</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" ht="44.200000000000003" customHeight="1">
+    <row r="6" ht="13.5">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" ht="68.200000000000003" customHeight="1">
+    <row r="7" ht="13.5">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" ht="68.200000000000003" customHeight="1">
+    <row r="8" ht="13.5">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" ht="56.200000000000003" customHeight="1">
+    <row r="9" ht="13.5">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" ht="56.200000000000003" customHeight="1">
+    <row r="10" ht="13.5">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" ht="44.200000000000003" customHeight="1">
+    <row r="11" ht="13.5">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" ht="44.200000000000003" customHeight="1">
+    <row r="12" ht="13.5">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" ht="44.200000000000003" customHeight="1">
+    <row r="13" ht="13.5">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" ht="56.200000000000003" customHeight="1">
+    <row r="14" ht="13.5">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" ht="44.200000000000003" customHeight="1">
+    <row r="15" ht="13.5">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="16" ht="56.200000000000003" customHeight="1">
+    <row r="16" ht="13.5">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" ht="68.200000000000003" customHeight="1">
+    <row r="17" ht="13.5">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" ht="56.200000000000003" customHeight="1">
+    <row r="18" ht="13.5">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="19" ht="56.200000000000003" customHeight="1">
+    <row r="19" ht="13.5">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" ht="20.199999999999999" customHeight="1">
+    <row r="20" ht="13.5">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="21" ht="44.200000000000003" customHeight="1">
+    <row r="21" ht="13.5">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" ht="44.200000000000003" customHeight="1">
+    <row r="22" ht="13.5">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="23" ht="44.200000000000003" customHeight="1">
+    <row r="23" ht="13.5">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="24" ht="56.200000000000003" customHeight="1">
+    <row r="24" ht="13.5">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="25" ht="104.2" customHeight="1">
+    <row r="25" ht="13.5">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="26" ht="92.200000000000003" customHeight="1">
+    <row r="26" ht="13.5">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="27" ht="68.200000000000003" customHeight="1">
+    <row r="27" ht="13.5">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="28" ht="80.200000000000003" customHeight="1">
+    <row r="28" ht="13.5">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="29" ht="44.200000000000003" customHeight="1">
+    <row r="29" ht="13.5">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" ht="80.200000000000003" customHeight="1">
+    <row r="30" ht="13.5">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="31" ht="56.200000000000003" customHeight="1">
+    <row r="31" ht="13.5">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="32" ht="44.200000000000003" customHeight="1">
+    <row r="32" ht="13.5">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="33" ht="56.200000000000003" customHeight="1">
+    <row r="33" ht="13.5">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="34" ht="32.200000000000003" customHeight="1">
+    <row r="34" ht="13.5">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="35" ht="68.200000000000003" customHeight="1">
+    <row r="35" ht="13.5">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="36" ht="32.200000000000003" customHeight="1">
+    <row r="36" ht="13.5">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="37" ht="44.200000000000003" customHeight="1">
+    <row r="37" ht="13.5">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="38" ht="44.200000000000003" customHeight="1">
+    <row r="38" ht="13.5">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="39" ht="32.200000000000003" customHeight="1">
+    <row r="39" ht="13.5">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="40" ht="44.200000000000003" customHeight="1">
+    <row r="40" ht="13.5">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="41" ht="56.200000000000003" customHeight="1">
+    <row r="41" ht="13.5">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="42" ht="56.200000000000003" customHeight="1">
+    <row r="42" ht="13.5">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -4388,7 +4388,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="43" ht="44.200000000000003" customHeight="1">
+    <row r="43" ht="13.5">
       <c r="A43" s="10">
         <v>42</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="44" ht="104.2" customHeight="1">
+    <row r="44" ht="13.5">
       <c r="A44" s="10">
         <v>43</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="45" ht="44.200000000000003" customHeight="1">
+    <row r="45" ht="13.5">
       <c r="A45" s="10">
         <v>44</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="46" ht="68.200000000000003" customHeight="1">
+    <row r="46" ht="13.5">
       <c r="A46" s="10">
         <v>45</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="47" ht="32.200000000000003" customHeight="1">
+    <row r="47" ht="13.5">
       <c r="A47" s="10">
         <v>46</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="48" ht="68.200000000000003" customHeight="1">
+    <row r="48" ht="13.5">
       <c r="A48" s="10">
         <v>47</v>
       </c>
@@ -4742,7 +4742,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="49" ht="68.200000000000003" customHeight="1">
+    <row r="49" ht="13.5">
       <c r="A49" s="10">
         <v>48</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="50" ht="68.200000000000003" customHeight="1">
+    <row r="50" ht="13.5">
       <c r="A50" s="10">
         <v>49</v>
       </c>
@@ -4860,7 +4860,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="51" ht="68.200000000000003" customHeight="1">
+    <row r="51" ht="13.5">
       <c r="A51" s="10">
         <v>50</v>
       </c>
@@ -4919,7 +4919,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="52" ht="80.200000000000003" customHeight="1">
+    <row r="52" ht="13.5">
       <c r="A52" s="10">
         <v>51</v>
       </c>
@@ -4978,7 +4978,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="53" ht="44.200000000000003" customHeight="1">
+    <row r="53" ht="13.5">
       <c r="A53" s="10">
         <v>52</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="54" ht="44.200000000000003" customHeight="1">
+    <row r="54" ht="13.5">
       <c r="A54" s="10">
         <v>53</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="55" ht="44.200000000000003" customHeight="1">
+    <row r="55" ht="13.5">
       <c r="A55" s="10">
         <v>54</v>
       </c>
@@ -5155,7 +5155,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="56" ht="32.200000000000003" customHeight="1">
+    <row r="56" ht="13.5">
       <c r="A56" s="10">
         <v>55</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="57" ht="140.19999999999999" customHeight="1">
+    <row r="57" ht="13.5">
       <c r="A57" s="10">
         <v>56</v>
       </c>
@@ -5273,7 +5273,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="58" ht="68.200000000000003" customHeight="1">
+    <row r="58" ht="13.5">
       <c r="A58" s="10">
         <v>57</v>
       </c>
@@ -5332,7 +5332,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="59" ht="20.199999999999999" customHeight="1">
+    <row r="59" ht="13.5">
       <c r="A59" s="10">
         <v>58</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="60" ht="20.199999999999999" customHeight="1">
+    <row r="60" ht="13.5">
       <c r="A60" s="15"/>
       <c r="B60" s="16"/>
       <c r="C60" s="17"/>

</xml_diff>

<commit_message>
working on 5-1 Trends
</commit_message>
<xml_diff>
--- a/tables/Simulatoren.xlsx
+++ b/tables/Simulatoren.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Cluster" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$T$58</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$T$58</definedName>
   </definedNames>
   <calcPr/>
@@ -1709,9 +1710,7 @@
     <col customWidth="1" min="1" max="1" style="1" width="5.3828100000000001"/>
     <col customWidth="1" min="2" max="6" style="1" width="16.351600000000001"/>
     <col customWidth="1" min="7" max="7" style="1" width="18.968800000000002"/>
-    <col customWidth="1" min="8" max="12" style="1" width="16.351600000000001"/>
-    <col customWidth="1" min="13" max="13" style="1" width="16.351600000000001"/>
-    <col customWidth="1" min="14" max="14" style="1" width="16.351600000000001"/>
+    <col customWidth="1" min="8" max="14" style="1" width="16.351600000000001"/>
     <col customWidth="1" min="15" max="20" style="1" width="19.5"/>
     <col customWidth="1" min="21" max="16384" style="1" width="16.351600000000001"/>
   </cols>
@@ -1778,7 +1777,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" ht="13.5">
+    <row r="2" ht="13.5" hidden="1">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1967,7 +1966,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" ht="13.5">
+    <row r="5" ht="13.5" hidden="1">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2030,7 +2029,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" ht="13.5">
+    <row r="6" ht="13.5" hidden="1">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2093,7 +2092,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" ht="13.5">
+    <row r="7" ht="13.5" hidden="1">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2156,7 +2155,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" ht="13.5">
+    <row r="8" ht="13.5" hidden="1">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2282,7 +2281,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" ht="13.5">
+    <row r="10" ht="13.5" hidden="1">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2534,7 +2533,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" ht="13.5">
+    <row r="14" ht="13.5" hidden="1">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2597,7 +2596,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" ht="13.5">
+    <row r="15" ht="13.5" hidden="1">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2660,7 +2659,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" ht="13.5">
+    <row r="16" ht="13.5" hidden="1">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2786,7 +2785,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" ht="13.5">
+    <row r="18" ht="13.5" hidden="1">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2975,7 +2974,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" ht="13.5">
+    <row r="21" ht="13.5" hidden="1">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -3038,7 +3037,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" ht="13.5">
+    <row r="22" ht="13.5" hidden="1">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -3101,7 +3100,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" ht="13.5">
+    <row r="23" ht="13.5" hidden="1">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -3164,7 +3163,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="24" ht="13.5">
+    <row r="24" ht="13.5" hidden="1">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -3227,7 +3226,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="25" ht="13.5">
+    <row r="25" ht="13.5" hidden="1">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -3290,7 +3289,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" ht="13.5">
+    <row r="26" ht="13.5" hidden="1">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -3353,7 +3352,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" ht="13.5">
+    <row r="27" ht="13.5" hidden="1">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -4928,7 +4927,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="52" ht="13.5">
+    <row r="52" ht="13.5" hidden="1">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -4991,7 +4990,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="53" ht="13.5">
+    <row r="53" ht="13.5" hidden="1">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -5054,7 +5053,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="54" ht="13.5">
+    <row r="54" ht="13.5" hidden="1">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -5117,7 +5116,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="55" ht="13.5">
+    <row r="55" ht="13.5" hidden="1">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -5180,7 +5179,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="56" ht="13.5">
+    <row r="56" ht="13.5" hidden="1">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -5243,7 +5242,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="57" ht="13.5">
+    <row r="57" ht="13.5" hidden="1">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -5306,7 +5305,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="58" ht="13.5">
+    <row r="58" ht="13.5" hidden="1">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -5392,7 +5391,14 @@
       <c r="T59" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T58"/>
+  <autoFilter ref="A1:T58">
+    <filterColumn colId="12">
+      <filters>
+        <filter val="Hardware und Logik"/>
+        <filter val="Prozessoren und Architekturen"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="T2" tooltip=""/>
     <hyperlink r:id="rId2" ref="T3" tooltip=""/>
@@ -5670,8 +5676,7 @@
     <col min="1" max="1" style="11" width="9.140625"/>
     <col customWidth="1" min="2" max="2" style="11" width="29.8515625"/>
     <col customWidth="1" min="3" max="3" style="11" width="38.28125"/>
-    <col min="4" max="4" style="11" width="9.140625"/>
-    <col min="5" max="16384" style="11" width="9.140625"/>
+    <col min="4" max="16384" style="11" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="3" ht="12.75">

</xml_diff>